<commit_message>
uploaded just snap caps
just snap caps uploaded for sale to distributors
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D0ED85-8B1F-422E-BEF9-BF2AC1E7F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21B8864-7603-40D8-9174-EE1D9173C1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="315" windowWidth="26295" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="465" windowWidth="15930" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="330">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -968,6 +968,48 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/htslabs/images/main/64435.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-black</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-black.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-blue</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-blue.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-gray</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-gray.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-green</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-green.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-pink</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-pink.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-red</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-red.jpg</t>
+  </si>
+  <si>
+    <t>snap-cap-yellow</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/snap-cap-yellow.jpg</t>
   </si>
 </sst>
 </file>
@@ -1826,15 +1868,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="72.85546875" customWidth="1"/>
   </cols>
@@ -3507,8 +3549,85 @@
       <c r="B152" s="1">
         <v>1212225</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="4" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>316</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>318</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>320</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>322</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>324</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>326</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>328</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3695,16 @@
     <hyperlink ref="C133" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="C34" r:id="rId62" xr:uid="{5AEA7608-B58A-4A60-A4AD-2AE2F5E780E9}"/>
     <hyperlink ref="C35" r:id="rId63" xr:uid="{AFE3A760-331C-44C9-BDA1-A87C0D227BE6}"/>
+    <hyperlink ref="C152" r:id="rId64" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
+    <hyperlink ref="C153" r:id="rId65" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
+    <hyperlink ref="C154" r:id="rId66" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
+    <hyperlink ref="C155" r:id="rId67" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
+    <hyperlink ref="C156" r:id="rId68" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
+    <hyperlink ref="C157" r:id="rId69" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
+    <hyperlink ref="C158" r:id="rId70" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
+    <hyperlink ref="C159" r:id="rId71" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId64"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added couple of wellplates
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5C812-57F2-4CD9-A77C-FAFFFD1DB32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D80984F-014F-4FA9-BFC5-BE3E63D1DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="735" windowWidth="28875" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="570" windowWidth="28875" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="364">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -1094,6 +1094,24 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/htslabs/images/main/931116-PORT-E.jpg</t>
+  </si>
+  <si>
+    <t>96-Well Plate, 2mL, Square Well, Round Bottom, Rim, Skirted, Raised Letters</t>
+  </si>
+  <si>
+    <t>96-Well Plate, 2mL, Square Well, V-Bottom, Raised Lettering, Sterile</t>
+  </si>
+  <si>
+    <t>951652B</t>
+  </si>
+  <si>
+    <t>951652C</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/951652B.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/951652C.jpg</t>
   </si>
 </sst>
 </file>
@@ -1952,15 +1970,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C168"/>
+  <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="1" max="1" width="68.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="72.85546875" customWidth="1"/>
   </cols>
@@ -3811,6 +3829,28 @@
       </c>
       <c r="C168" s="4" t="s">
         <v>324</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>358</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>359</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3896,8 +3936,10 @@
     <hyperlink ref="C64" r:id="rId79" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
     <hyperlink ref="C65" r:id="rId80" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
     <hyperlink ref="C66" r:id="rId81" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
+    <hyperlink ref="C169" r:id="rId82" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
+    <hyperlink ref="C170" r:id="rId83" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId82"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId84"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some std and the whole x44 wxtreme
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297B6D85-EAA7-4499-9A85-0E8F5456DCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CD5749-B4D5-4F50-8A22-60B7603AB5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="570" windowWidth="28875" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="765" windowWidth="21375" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="376">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -1112,6 +1112,42 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/htslabs/images/main/951652C.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/34439.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/34438.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/34435.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/34441.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/34431.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84430.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84440.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84431.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84441.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84435.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84438.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/84439.jpg</t>
   </si>
 </sst>
 </file>
@@ -1970,10 +2006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,1895 +2087,2039 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" s="1">
-        <v>35541</v>
+        <v>34431</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>125</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="1">
-        <v>35535</v>
+        <v>35541</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B9" s="1">
-        <v>35538</v>
+        <v>34441</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>127</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B10" s="1">
-        <v>35539</v>
-      </c>
-      <c r="C10" t="s">
-        <v>128</v>
+        <v>35535</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B11" s="1">
-        <v>15530</v>
-      </c>
-      <c r="C11" t="s">
-        <v>129</v>
+        <v>34435</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B12" s="1">
-        <v>15540</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
+        <v>35538</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B13" s="1">
-        <v>15531</v>
-      </c>
-      <c r="C13" t="s">
-        <v>131</v>
+        <v>34438</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B14" s="1">
-        <v>25530</v>
+        <v>35539</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B15" s="1">
-        <v>25540</v>
-      </c>
-      <c r="C15" t="s">
-        <v>133</v>
+        <v>34439</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B16" s="1">
-        <v>25531</v>
+        <v>15530</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B17" s="1">
-        <v>15541</v>
+        <v>15540</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18" s="1">
-        <v>25541</v>
+        <v>15531</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B19" s="1">
-        <v>15535</v>
+        <v>25530</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B20" s="1">
-        <v>25535</v>
+        <v>25540</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B21" s="1">
-        <v>15538</v>
+        <v>25531</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B22" s="1">
-        <v>25538</v>
+        <v>15541</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B23" s="1">
-        <v>14930</v>
+        <v>25541</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B24" s="1">
-        <v>85530</v>
+        <v>15535</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B25" s="1">
-        <v>85540</v>
+        <v>25535</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B26" s="1">
-        <v>85531</v>
+        <v>15538</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B27" s="1">
-        <v>85541</v>
+        <v>25538</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B28" s="1">
-        <v>85535</v>
+        <v>14930</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B29" s="1">
-        <v>85538</v>
+        <v>85530</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B30" s="1">
-        <v>85539</v>
+        <v>85540</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="B31" s="1">
-        <v>64430</v>
+        <v>85531</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="B32" s="1">
-        <v>64440</v>
+        <v>85541</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="B33" s="1">
-        <v>64431</v>
+        <v>85535</v>
       </c>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="B34" s="1">
-        <v>64441</v>
+        <v>85538</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="B35" s="1">
-        <v>64438</v>
+        <v>85539</v>
       </c>
       <c r="C35" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B36" s="1">
-        <v>64439</v>
+        <v>84430</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>154</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>310</v>
+        <v>247</v>
       </c>
       <c r="B37" s="1">
-        <v>64435</v>
+        <v>84440</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>311</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="B38" s="1">
-        <v>35005</v>
-      </c>
-      <c r="C38" t="s">
-        <v>155</v>
+        <v>84431</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>249</v>
       </c>
       <c r="B39" s="1">
-        <v>35015</v>
-      </c>
-      <c r="C39" t="s">
-        <v>156</v>
+        <v>84441</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>253</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>250</v>
+      </c>
+      <c r="B40" s="1">
+        <v>84435</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>373</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>254</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>2</v>
+        <v>251</v>
+      </c>
+      <c r="B41" s="1">
+        <v>84438</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>218</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>255</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>3</v>
+        <v>252</v>
+      </c>
+      <c r="B42" s="1">
+        <v>84439</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>219</v>
+        <v>375</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>256</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>220</v>
+        <v>231</v>
+      </c>
+      <c r="B43" s="1">
+        <v>64430</v>
+      </c>
+      <c r="C43" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>257</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>221</v>
+        <v>232</v>
+      </c>
+      <c r="B44" s="1">
+        <v>64440</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>258</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>222</v>
+        <v>233</v>
+      </c>
+      <c r="B45" s="1">
+        <v>64431</v>
+      </c>
+      <c r="C45" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1">
-        <v>9452099</v>
+        <v>64441</v>
       </c>
       <c r="C46" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>260</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>223</v>
+        <v>235</v>
+      </c>
+      <c r="B47" s="1">
+        <v>64438</v>
+      </c>
+      <c r="C47" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>236</v>
       </c>
       <c r="B48" s="1">
-        <v>235008</v>
-      </c>
-      <c r="C48" t="s">
-        <v>158</v>
+        <v>64439</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="B49" s="1">
-        <v>491250</v>
-      </c>
-      <c r="C49" t="s">
-        <v>159</v>
+        <v>64435</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="B50" s="1">
-        <v>491252</v>
+        <v>35005</v>
       </c>
       <c r="C50" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>263</v>
+        <v>1</v>
       </c>
       <c r="B51" s="1">
-        <v>491253</v>
+        <v>35015</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>264</v>
-      </c>
-      <c r="B52" s="1">
-        <v>491254</v>
-      </c>
-      <c r="C52" t="s">
-        <v>162</v>
+        <v>253</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>265</v>
-      </c>
-      <c r="B53" s="1">
-        <v>491256</v>
-      </c>
-      <c r="C53" t="s">
-        <v>163</v>
+        <v>254</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>266</v>
-      </c>
-      <c r="B54" s="1">
-        <v>491258</v>
-      </c>
-      <c r="C54" t="s">
-        <v>164</v>
+        <v>255</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>267</v>
-      </c>
-      <c r="B55" s="1">
-        <v>491260</v>
-      </c>
-      <c r="C55" t="s">
-        <v>165</v>
+        <v>256</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>268</v>
-      </c>
-      <c r="B56" s="1">
-        <v>931110</v>
-      </c>
-      <c r="C56" t="s">
-        <v>166</v>
+        <v>257</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>269</v>
-      </c>
-      <c r="B57" s="1">
-        <v>931111</v>
-      </c>
-      <c r="C57" t="s">
-        <v>167</v>
+        <v>258</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B58" s="1">
-        <v>931112</v>
+        <v>9452099</v>
       </c>
       <c r="C58" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>271</v>
-      </c>
-      <c r="B59" s="1">
-        <v>931113</v>
-      </c>
-      <c r="C59" t="s">
-        <v>169</v>
+        <v>260</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>272</v>
+        <v>8</v>
       </c>
       <c r="B60" s="1">
-        <v>931114</v>
+        <v>235008</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B61" s="1">
-        <v>931116</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>89</v>
+        <v>491250</v>
+      </c>
+      <c r="C61" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>336</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>331</v>
+        <v>262</v>
+      </c>
+      <c r="B62" s="1">
+        <v>491252</v>
+      </c>
+      <c r="C62" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>337</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>332</v>
+        <v>263</v>
+      </c>
+      <c r="B63" s="1">
+        <v>491253</v>
+      </c>
+      <c r="C63" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>338</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>333</v>
+        <v>264</v>
+      </c>
+      <c r="B64" s="1">
+        <v>491254</v>
+      </c>
+      <c r="C64" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>339</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>334</v>
+        <v>265</v>
+      </c>
+      <c r="B65" s="1">
+        <v>491256</v>
+      </c>
+      <c r="C65" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>340</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>335</v>
+        <v>266</v>
+      </c>
+      <c r="B66" s="1">
+        <v>491258</v>
+      </c>
+      <c r="C66" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>341</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>89</v>
+        <v>267</v>
+      </c>
+      <c r="B67" s="1">
+        <v>491260</v>
+      </c>
+      <c r="C67" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>274</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>356</v>
+        <v>268</v>
+      </c>
+      <c r="B68" s="1">
+        <v>931110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>275</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>88</v>
+        <v>269</v>
+      </c>
+      <c r="B69" s="1">
+        <v>931111</v>
+      </c>
+      <c r="C69" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>276</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>87</v>
+        <v>270</v>
+      </c>
+      <c r="B70" s="1">
+        <v>931112</v>
+      </c>
+      <c r="C70" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>277</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>357</v>
+        <v>271</v>
+      </c>
+      <c r="B71" s="1">
+        <v>931113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>278</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>106</v>
+        <v>272</v>
+      </c>
+      <c r="B72" s="1">
+        <v>931114</v>
+      </c>
+      <c r="C72" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>279</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>12</v>
+        <v>273</v>
+      </c>
+      <c r="B73" s="1">
+        <v>931116</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>280</v>
+        <v>336</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>13</v>
+        <v>325</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>108</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>281</v>
+        <v>337</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>14</v>
+        <v>326</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>109</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>15</v>
+        <v>327</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>110</v>
+        <v>333</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B77" s="1">
-        <v>1212900</v>
+        <v>339</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>86</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>17</v>
-      </c>
-      <c r="B78" s="1">
-        <v>1212905</v>
+        <v>340</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>85</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>283</v>
-      </c>
-      <c r="B79" s="1">
-        <v>899110</v>
+        <v>341</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>284</v>
-      </c>
-      <c r="B80" s="1">
-        <v>899111</v>
+        <v>274</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>83</v>
+        <v>356</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>285</v>
-      </c>
-      <c r="B81" s="1">
-        <v>899112</v>
+        <v>275</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>286</v>
-      </c>
-      <c r="B82" s="1">
-        <v>899116</v>
+        <v>276</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>80</v>
+        <v>357</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>278</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>288</v>
-      </c>
-      <c r="B85" s="1">
-        <v>788116</v>
-      </c>
-      <c r="C85" t="s">
-        <v>171</v>
+        <v>279</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>289</v>
-      </c>
-      <c r="B86" s="1">
-        <v>931147</v>
-      </c>
-      <c r="C86" t="s">
-        <v>172</v>
+        <v>280</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>290</v>
-      </c>
-      <c r="B87" s="1">
-        <v>931144</v>
-      </c>
-      <c r="C87" t="s">
-        <v>173</v>
+        <v>281</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>291</v>
-      </c>
-      <c r="B88" s="1">
-        <v>931141</v>
-      </c>
-      <c r="C88" t="s">
-        <v>174</v>
+        <v>282</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>16</v>
       </c>
       <c r="B89" s="1">
-        <v>931138</v>
+        <v>1212900</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>293</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1212905</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B91" s="1">
-        <v>899136</v>
+        <v>899110</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B92" s="1">
-        <v>899109</v>
+        <v>899111</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B93" s="1">
-        <v>899110</v>
+        <v>899112</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B94" s="1">
-        <v>899111</v>
+        <v>899116</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>298</v>
-      </c>
-      <c r="B95" s="1">
-        <v>899566</v>
+        <v>287</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>299</v>
-      </c>
-      <c r="B96" s="1">
-        <v>899421</v>
+        <v>18</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B97" s="1">
-        <v>899423</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>117</v>
+        <v>788116</v>
+      </c>
+      <c r="C97" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B98" s="1">
-        <v>899424</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>118</v>
+        <v>931147</v>
+      </c>
+      <c r="C98" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B99" s="1">
-        <v>899425</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>119</v>
+        <v>931144</v>
+      </c>
+      <c r="C99" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B100" s="1">
-        <v>446300</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>120</v>
+        <v>931141</v>
+      </c>
+      <c r="C100" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>301</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>21</v>
+        <v>292</v>
+      </c>
+      <c r="B101" s="1">
+        <v>931138</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>301</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>23</v>
+        <v>294</v>
+      </c>
+      <c r="B103" s="1">
+        <v>899136</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>301</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>24</v>
+        <v>295</v>
+      </c>
+      <c r="B104" s="1">
+        <v>899109</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>302</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>25</v>
+        <v>296</v>
+      </c>
+      <c r="B105" s="1">
+        <v>899110</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>302</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>26</v>
+        <v>297</v>
+      </c>
+      <c r="B106" s="1">
+        <v>899111</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>302</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>27</v>
+        <v>298</v>
+      </c>
+      <c r="B107" s="1">
+        <v>899566</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>302</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>28</v>
+        <v>299</v>
+      </c>
+      <c r="B108" s="1">
+        <v>899421</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>302</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>29</v>
+        <v>299</v>
+      </c>
+      <c r="B109" s="1">
+        <v>899423</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>303</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>30</v>
+        <v>299</v>
+      </c>
+      <c r="B110" s="1">
+        <v>899424</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>303</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>31</v>
+        <v>299</v>
+      </c>
+      <c r="B111" s="1">
+        <v>899425</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>304</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>32</v>
+        <v>300</v>
+      </c>
+      <c r="B112" s="1">
+        <v>446300</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>306</v>
-      </c>
-      <c r="B115" s="1">
-        <v>931609</v>
-      </c>
-      <c r="C115" t="s">
-        <v>175</v>
+        <v>301</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>307</v>
-      </c>
-      <c r="B116" s="1">
-        <v>931700</v>
-      </c>
-      <c r="C116" t="s">
-        <v>176</v>
+        <v>301</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>308</v>
-      </c>
-      <c r="B117" s="1">
-        <v>931606</v>
-      </c>
-      <c r="C117" t="s">
-        <v>177</v>
+        <v>302</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>309</v>
-      </c>
-      <c r="B118" s="1">
-        <v>931607</v>
-      </c>
-      <c r="C118" t="s">
-        <v>178</v>
+        <v>302</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>35</v>
+        <v>302</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C119" t="s">
-        <v>179</v>
+        <v>27</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>35</v>
-      </c>
-      <c r="B120" s="1">
-        <v>931568</v>
-      </c>
-      <c r="C120" t="s">
-        <v>180</v>
+        <v>302</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>302</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C121" t="s">
-        <v>181</v>
+        <v>29</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>37</v>
-      </c>
-      <c r="B122" s="1">
-        <v>931571</v>
-      </c>
-      <c r="C122" t="s">
-        <v>182</v>
+        <v>303</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>39</v>
-      </c>
-      <c r="B123" s="1">
-        <v>951657</v>
-      </c>
-      <c r="C123" t="s">
-        <v>183</v>
+        <v>303</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>39</v>
+        <v>304</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>39</v>
-      </c>
-      <c r="B125" s="1">
-        <v>931130</v>
-      </c>
-      <c r="C125" t="s">
-        <v>184</v>
+        <v>305</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>305</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C126" t="s">
-        <v>185</v>
+        <v>34</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>237</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>42</v>
+        <v>306</v>
+      </c>
+      <c r="B127" s="1">
+        <v>931609</v>
       </c>
       <c r="C127" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>238</v>
+        <v>307</v>
       </c>
       <c r="B128" s="1">
-        <v>9356045</v>
+        <v>931700</v>
       </c>
       <c r="C128" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>39</v>
+        <v>308</v>
       </c>
       <c r="B129" s="1">
-        <v>931133</v>
+        <v>931606</v>
       </c>
       <c r="C129" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>39</v>
+        <v>309</v>
       </c>
       <c r="B130" s="1">
-        <v>931137</v>
+        <v>931607</v>
       </c>
       <c r="C130" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>43</v>
-      </c>
-      <c r="B131" s="1">
-        <v>931919</v>
+        <v>35</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C131" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B132" s="1">
-        <v>921746</v>
+        <v>931568</v>
       </c>
       <c r="C132" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>43</v>
-      </c>
-      <c r="B133" s="1">
-        <v>921730</v>
+        <v>37</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C133" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B134" s="1">
-        <v>921740</v>
+        <v>931571</v>
       </c>
       <c r="C134" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B135" s="1">
-        <v>921731</v>
+        <v>951657</v>
       </c>
       <c r="C135" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>44</v>
-      </c>
-      <c r="B136" s="1">
-        <v>921550</v>
-      </c>
-      <c r="C136" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B137" s="1">
-        <v>921546</v>
+        <v>931130</v>
       </c>
       <c r="C137" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>46</v>
-      </c>
-      <c r="B138" s="1">
-        <v>359747</v>
+        <v>39</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C138" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C139" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>48</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>199</v>
+        <v>238</v>
+      </c>
+      <c r="B140" s="1">
+        <v>9356045</v>
+      </c>
+      <c r="C140" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B141" s="1">
-        <v>899410</v>
+        <v>931133</v>
       </c>
       <c r="C141" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B142" s="1">
-        <v>899403</v>
+        <v>931137</v>
       </c>
       <c r="C142" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B143" s="1">
-        <v>899406</v>
+        <v>931919</v>
       </c>
       <c r="C143" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B144" s="1">
-        <v>981945</v>
+        <v>921746</v>
       </c>
       <c r="C144" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B145" s="1">
-        <v>981948</v>
+        <v>921730</v>
       </c>
       <c r="C145" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B146" s="1">
-        <v>981802</v>
+        <v>921740</v>
       </c>
       <c r="C146" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B147" s="1">
-        <v>205410</v>
+        <v>921731</v>
       </c>
       <c r="C147" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B148" s="1">
-        <v>402805</v>
+        <v>921550</v>
       </c>
       <c r="C148" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>58</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="B149" s="1">
+        <v>921546</v>
       </c>
       <c r="C149" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>239</v>
+        <v>46</v>
       </c>
       <c r="B150" s="1">
-        <v>30312</v>
+        <v>359747</v>
       </c>
       <c r="C150" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>60</v>
-      </c>
-      <c r="B151" s="1">
-        <v>70502</v>
+        <v>46</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C151" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>60</v>
-      </c>
-      <c r="B152" s="1">
-        <v>70512</v>
-      </c>
-      <c r="C152" t="s">
-        <v>211</v>
+        <v>48</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>61</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>212</v>
+        <v>50</v>
+      </c>
+      <c r="B153" s="1">
+        <v>899410</v>
+      </c>
+      <c r="C153" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B154" s="1">
-        <v>1212280</v>
+        <v>899403</v>
       </c>
       <c r="C154" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>64</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="B155" s="1">
+        <v>899406</v>
       </c>
       <c r="C155" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>66</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="B156" s="1">
+        <v>981945</v>
       </c>
       <c r="C156" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>68</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>90</v>
+        <v>54</v>
+      </c>
+      <c r="B157" s="1">
+        <v>981948</v>
+      </c>
+      <c r="C157" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B158" s="1">
-        <v>1212085</v>
+        <v>981802</v>
       </c>
       <c r="C158" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B159" s="1">
-        <v>1212225</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>217</v>
+        <v>205410</v>
+      </c>
+      <c r="C159" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>312</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>344</v>
+        <v>57</v>
+      </c>
+      <c r="B160" s="1">
+        <v>402805</v>
+      </c>
+      <c r="C160" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>313</v>
+        <v>58</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>343</v>
+        <v>59</v>
+      </c>
+      <c r="C161" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>314</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>349</v>
+        <v>239</v>
+      </c>
+      <c r="B162" s="1">
+        <v>30312</v>
+      </c>
+      <c r="C162" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>315</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>347</v>
+        <v>60</v>
+      </c>
+      <c r="B163" s="1">
+        <v>70502</v>
+      </c>
+      <c r="C163" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>316</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C164" s="4" t="s">
-        <v>351</v>
+        <v>60</v>
+      </c>
+      <c r="B164" s="1">
+        <v>70512</v>
+      </c>
+      <c r="C164" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>317</v>
+        <v>61</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>352</v>
+        <v>62</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>353</v>
+        <v>212</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>318</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>355</v>
+        <v>63</v>
+      </c>
+      <c r="B166" s="1">
+        <v>1212280</v>
+      </c>
+      <c r="C166" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>321</v>
-      </c>
-      <c r="B167" s="1">
-        <v>70680</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>322</v>
+        <v>64</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C167" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>323</v>
-      </c>
-      <c r="B168" s="1">
-        <v>14638</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>324</v>
+        <v>66</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C168" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>358</v>
+        <v>68</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>360</v>
+        <v>69</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>362</v>
+        <v>90</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>70</v>
+      </c>
+      <c r="B170" s="1">
+        <v>1212085</v>
+      </c>
+      <c r="C170" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>71</v>
+      </c>
+      <c r="B171" s="1">
+        <v>1212225</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>313</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>314</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>315</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>316</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>317</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>318</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>321</v>
+      </c>
+      <c r="B179" s="1">
+        <v>70680</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>323</v>
+      </c>
+      <c r="B180" s="1">
+        <v>14638</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>358</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>359</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B182" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C182" s="4" t="s">
         <v>363</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C40" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C71" r:id="rId2" display="https://raw.githubusercontent.com/htslabs/images/main/ 931116-PORT-E.jpg" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C68" r:id="rId3" display="https://raw.githubusercontent.com/htslabs/images/main/ 931110-SP.jpg" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C83" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C82" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C81" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C80" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C79" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C78" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C77" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C70" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C69" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C61" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C157" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C124" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C113" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C112" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C111" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C110" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C101" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C102" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C104" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C105" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C106" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C107" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C108" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C109" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C103" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C114" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C72" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C73" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C74" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C75" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C76" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C84" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C90" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C91" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C92" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C93" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C94" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C95" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C96" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C97" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C98" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C99" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C100" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C89" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C83" r:id="rId2" display="https://raw.githubusercontent.com/htslabs/images/main/ 931116-PORT-E.jpg" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C80" r:id="rId3" display="https://raw.githubusercontent.com/htslabs/images/main/ 931110-SP.jpg" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C95" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C94" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C93" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C92" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C91" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C90" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C89" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C82" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C81" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C73" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C169" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C136" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C125" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C124" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C123" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C122" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C113" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C114" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C116" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C117" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C118" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C119" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C120" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C121" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C115" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C126" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C84" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C85" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C86" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C87" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C88" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C96" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C102" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C103" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C104" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C105" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C106" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C107" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C108" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C109" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C110" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C111" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C112" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C101" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="C4" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="C5" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="C6" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C7" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C8" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C9" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C41" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C42" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C43" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C44" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C45" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C47" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C153" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C140" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C36" r:id="rId62" xr:uid="{5AEA7608-B58A-4A60-A4AD-2AE2F5E780E9}"/>
-    <hyperlink ref="C37" r:id="rId63" xr:uid="{AFE3A760-331C-44C9-BDA1-A87C0D227BE6}"/>
-    <hyperlink ref="C159" r:id="rId64" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
-    <hyperlink ref="C160" r:id="rId65" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
-    <hyperlink ref="C161" r:id="rId66" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
-    <hyperlink ref="C162" r:id="rId67" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
-    <hyperlink ref="C163" r:id="rId68" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
-    <hyperlink ref="C164" r:id="rId69" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
-    <hyperlink ref="C165" r:id="rId70" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
-    <hyperlink ref="C166" r:id="rId71" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
-    <hyperlink ref="C2" r:id="rId72" xr:uid="{55A7AC5D-4A55-40FD-B555-BF115B8C3DB2}"/>
-    <hyperlink ref="C3" r:id="rId73" xr:uid="{5B2A9690-E72E-4F75-AE57-C9AB31B6BDD8}"/>
-    <hyperlink ref="C167" r:id="rId74" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
-    <hyperlink ref="C168" r:id="rId75" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
-    <hyperlink ref="C67" r:id="rId76" xr:uid="{73ED57B4-3A6D-4846-9BEA-15F1B2FCC3F8}"/>
-    <hyperlink ref="C62" r:id="rId77" xr:uid="{DD8214E1-24DE-4AF8-BCA7-B2D42CBE725C}"/>
-    <hyperlink ref="C63" r:id="rId78" xr:uid="{A5FD4093-9D9B-431D-A285-90214E03180A}"/>
-    <hyperlink ref="C64" r:id="rId79" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
-    <hyperlink ref="C65" r:id="rId80" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
-    <hyperlink ref="C66" r:id="rId81" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
-    <hyperlink ref="C169" r:id="rId82" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
-    <hyperlink ref="C170" r:id="rId83" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
+    <hyperlink ref="C10" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C12" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C53" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C54" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C55" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C57" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C165" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C152" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C48" r:id="rId61" xr:uid="{5AEA7608-B58A-4A60-A4AD-2AE2F5E780E9}"/>
+    <hyperlink ref="C49" r:id="rId62" xr:uid="{AFE3A760-331C-44C9-BDA1-A87C0D227BE6}"/>
+    <hyperlink ref="C171" r:id="rId63" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
+    <hyperlink ref="C172" r:id="rId64" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
+    <hyperlink ref="C173" r:id="rId65" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
+    <hyperlink ref="C174" r:id="rId66" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
+    <hyperlink ref="C175" r:id="rId67" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
+    <hyperlink ref="C176" r:id="rId68" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
+    <hyperlink ref="C177" r:id="rId69" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
+    <hyperlink ref="C178" r:id="rId70" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
+    <hyperlink ref="C2" r:id="rId71" xr:uid="{55A7AC5D-4A55-40FD-B555-BF115B8C3DB2}"/>
+    <hyperlink ref="C3" r:id="rId72" xr:uid="{5B2A9690-E72E-4F75-AE57-C9AB31B6BDD8}"/>
+    <hyperlink ref="C179" r:id="rId73" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
+    <hyperlink ref="C180" r:id="rId74" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
+    <hyperlink ref="C79" r:id="rId75" xr:uid="{73ED57B4-3A6D-4846-9BEA-15F1B2FCC3F8}"/>
+    <hyperlink ref="C74" r:id="rId76" xr:uid="{DD8214E1-24DE-4AF8-BCA7-B2D42CBE725C}"/>
+    <hyperlink ref="C75" r:id="rId77" xr:uid="{A5FD4093-9D9B-431D-A285-90214E03180A}"/>
+    <hyperlink ref="C76" r:id="rId78" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
+    <hyperlink ref="C77" r:id="rId79" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
+    <hyperlink ref="C78" r:id="rId80" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
+    <hyperlink ref="C181" r:id="rId81" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
+    <hyperlink ref="C182" r:id="rId82" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
+    <hyperlink ref="C8" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C15" r:id="rId84" xr:uid="{D53AF88A-6A97-43F1-9E72-EFA6A2CDA035}"/>
+    <hyperlink ref="C13" r:id="rId85" xr:uid="{B8D33A38-937A-4646-A6A0-6215623CD68F}"/>
+    <hyperlink ref="C11" r:id="rId86" xr:uid="{37DE3B9A-ABE2-4AD2-9D08-717600B8E4DA}"/>
+    <hyperlink ref="C9" r:id="rId87" xr:uid="{6F3766C2-12D3-4F36-AFCD-9065EA35D3E7}"/>
+    <hyperlink ref="C7" r:id="rId88" xr:uid="{1BBCF9BC-DB48-4BF6-838A-208E9F9A8847}"/>
+    <hyperlink ref="C36" r:id="rId89" xr:uid="{F11189E3-8C38-413A-8BCE-2ABAE14AF6D3}"/>
+    <hyperlink ref="C37" r:id="rId90" xr:uid="{56968528-F69B-40F3-8275-DAE7ADFF6D1C}"/>
+    <hyperlink ref="C38" r:id="rId91" xr:uid="{26BA8B92-C5CF-47DC-8679-82D3D996E6C0}"/>
+    <hyperlink ref="C39" r:id="rId92" xr:uid="{4D26C214-DDF0-49D3-9EB8-CC5EA5B25C2A}"/>
+    <hyperlink ref="C40" r:id="rId93" xr:uid="{A68412B5-9C33-485D-ADE1-B208669B4ACE}"/>
+    <hyperlink ref="C41" r:id="rId94" xr:uid="{B0C47993-5B25-4EEA-AC00-BD9C1AD317C5}"/>
+    <hyperlink ref="C42" r:id="rId95" xr:uid="{350F7192-A024-4641-BFDD-8597950B5A03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId84"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId96"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6 well and 7L added
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F4E2D2-EBAC-4843-8E2B-E1C749E34923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACD2ED-CCBB-4EA4-819D-C36B81E47DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="465" windowWidth="31530" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1005" windowWidth="35880" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="390">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -1166,6 +1166,30 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/htslabs/images/main/931110-11.jpg</t>
+  </si>
+  <si>
+    <t>Optimum Growth® 7L Flask</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931117.jpg</t>
+  </si>
+  <si>
+    <t>Optimum Growth® 7L Flask double-bagged</t>
+  </si>
+  <si>
+    <t>931117-DB</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931117-DB.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931116-DB.jpg</t>
+  </si>
+  <si>
+    <t>6-Well Plate, w/Lid</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931167.jpg</t>
   </si>
 </sst>
 </file>
@@ -2034,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2852,420 +2876,420 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>336</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>325</v>
+        <v>382</v>
+      </c>
+      <c r="B74" s="1">
+        <v>931117</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>331</v>
+        <v>383</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>380</v>
+        <v>329</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>381</v>
+        <v>335</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>341</v>
+        <v>379</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>330</v>
+        <v>380</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>89</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>274</v>
+        <v>341</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>330</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>384</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>77</v>
+        <v>385</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>88</v>
+        <v>386</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>87</v>
+        <v>356</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>357</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>107</v>
+        <v>357</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>377</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>376</v>
+        <v>280</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>378</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>16</v>
-      </c>
-      <c r="B91" s="1">
-        <v>1212900</v>
+        <v>377</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>376</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>86</v>
+        <v>378</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>17</v>
-      </c>
-      <c r="B92" s="1">
-        <v>1212905</v>
+        <v>282</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>283</v>
+        <v>16</v>
       </c>
       <c r="B93" s="1">
-        <v>899110</v>
+        <v>1212900</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="B94" s="1">
-        <v>899111</v>
+        <v>1212905</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B95" s="1">
-        <v>899112</v>
+        <v>899110</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B96" s="1">
-        <v>899116</v>
+        <v>899111</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>287</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>79</v>
+        <v>285</v>
+      </c>
+      <c r="B97" s="1">
+        <v>899112</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>18</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>19</v>
+        <v>286</v>
+      </c>
+      <c r="B98" s="1">
+        <v>899116</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>288</v>
-      </c>
-      <c r="B99" s="1">
-        <v>788116</v>
-      </c>
-      <c r="C99" t="s">
-        <v>171</v>
+        <v>287</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>289</v>
-      </c>
-      <c r="B100" s="1">
-        <v>931147</v>
-      </c>
-      <c r="C100" t="s">
-        <v>172</v>
+        <v>18</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B101" s="1">
-        <v>931144</v>
+        <v>788116</v>
       </c>
       <c r="C101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B102" s="1">
-        <v>931141</v>
+        <v>931147</v>
       </c>
       <c r="C102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B103" s="1">
-        <v>931138</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>121</v>
+        <v>931144</v>
+      </c>
+      <c r="C103" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>293</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>112</v>
+        <v>291</v>
+      </c>
+      <c r="B104" s="1">
+        <v>931141</v>
+      </c>
+      <c r="C104" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B105" s="1">
-        <v>899136</v>
+        <v>931138</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>295</v>
-      </c>
-      <c r="B106" s="1">
-        <v>899109</v>
+        <v>293</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B107" s="1">
-        <v>899110</v>
+        <v>899136</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B108" s="1">
-        <v>899111</v>
+        <v>899109</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B109" s="1">
-        <v>899566</v>
+        <v>899110</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B110" s="1">
-        <v>899421</v>
+        <v>899111</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B111" s="1">
-        <v>899423</v>
+        <v>899566</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3273,10 +3297,10 @@
         <v>299</v>
       </c>
       <c r="B112" s="1">
-        <v>899424</v>
+        <v>899421</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3284,43 +3308,43 @@
         <v>299</v>
       </c>
       <c r="B113" s="1">
-        <v>899425</v>
+        <v>899423</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B114" s="1">
-        <v>446300</v>
+        <v>899424</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>301</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>21</v>
+        <v>299</v>
+      </c>
+      <c r="B115" s="1">
+        <v>899425</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>301</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>22</v>
+        <v>300</v>
+      </c>
+      <c r="B116" s="1">
+        <v>446300</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3328,10 +3352,10 @@
         <v>301</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3339,32 +3363,32 @@
         <v>301</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3372,10 +3396,10 @@
         <v>302</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3383,10 +3407,10 @@
         <v>302</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3394,175 +3418,175 @@
         <v>302</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>306</v>
-      </c>
-      <c r="B129" s="1">
-        <v>931609</v>
-      </c>
-      <c r="C129" t="s">
-        <v>175</v>
+        <v>305</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>307</v>
-      </c>
-      <c r="B130" s="1">
-        <v>931700</v>
-      </c>
-      <c r="C130" t="s">
-        <v>176</v>
+        <v>305</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B131" s="1">
-        <v>931606</v>
+        <v>931609</v>
       </c>
       <c r="C131" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B132" s="1">
-        <v>931607</v>
+        <v>931700</v>
       </c>
       <c r="C132" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>35</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>36</v>
+        <v>308</v>
+      </c>
+      <c r="B133" s="1">
+        <v>931606</v>
       </c>
       <c r="C133" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>35</v>
+        <v>309</v>
       </c>
       <c r="B134" s="1">
-        <v>931568</v>
+        <v>931607</v>
       </c>
       <c r="C134" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C135" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B136" s="1">
-        <v>931571</v>
+        <v>931568</v>
       </c>
       <c r="C136" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>39</v>
-      </c>
-      <c r="B137" s="1">
-        <v>951657</v>
+        <v>37</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C137" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>39</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>91</v>
+        <v>37</v>
+      </c>
+      <c r="B138" s="1">
+        <v>931571</v>
+      </c>
+      <c r="C138" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -3570,10 +3594,10 @@
         <v>39</v>
       </c>
       <c r="B139" s="1">
-        <v>931130</v>
+        <v>951657</v>
       </c>
       <c r="C139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3581,76 +3605,76 @@
         <v>39</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C140" t="s">
-        <v>185</v>
+        <v>40</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>237</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="B141" s="1">
+        <v>931130</v>
       </c>
       <c r="C141" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>238</v>
-      </c>
-      <c r="B142" s="1">
-        <v>9356045</v>
+        <v>39</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C142" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>39</v>
-      </c>
-      <c r="B143" s="1">
-        <v>931133</v>
+        <v>237</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C143" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
       <c r="B144" s="1">
-        <v>931137</v>
+        <v>9356045</v>
       </c>
       <c r="C144" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B145" s="1">
-        <v>931919</v>
+        <v>931133</v>
       </c>
       <c r="C145" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B146" s="1">
-        <v>921746</v>
+        <v>931137</v>
       </c>
       <c r="C146" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3658,10 +3682,10 @@
         <v>43</v>
       </c>
       <c r="B147" s="1">
-        <v>921730</v>
+        <v>931919</v>
       </c>
       <c r="C147" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3669,10 +3693,10 @@
         <v>43</v>
       </c>
       <c r="B148" s="1">
-        <v>921740</v>
+        <v>921746</v>
       </c>
       <c r="C148" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3680,446 +3704,479 @@
         <v>43</v>
       </c>
       <c r="B149" s="1">
-        <v>921731</v>
+        <v>921730</v>
       </c>
       <c r="C149" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B150" s="1">
-        <v>921550</v>
+        <v>921740</v>
       </c>
       <c r="C150" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B151" s="1">
-        <v>921546</v>
+        <v>921731</v>
       </c>
       <c r="C151" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B152" s="1">
-        <v>359747</v>
+        <v>921550</v>
       </c>
       <c r="C152" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>46</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B153" s="1">
+        <v>921546</v>
       </c>
       <c r="C153" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>48</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>199</v>
+        <v>46</v>
+      </c>
+      <c r="B154" s="1">
+        <v>359747</v>
+      </c>
+      <c r="C154" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>50</v>
-      </c>
-      <c r="B155" s="1">
-        <v>899410</v>
+        <v>46</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C155" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>51</v>
-      </c>
-      <c r="B156" s="1">
-        <v>899403</v>
-      </c>
-      <c r="C156" t="s">
-        <v>201</v>
+        <v>48</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B157" s="1">
-        <v>899406</v>
+        <v>899410</v>
       </c>
       <c r="C157" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B158" s="1">
-        <v>981945</v>
+        <v>899403</v>
       </c>
       <c r="C158" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B159" s="1">
-        <v>981948</v>
+        <v>899406</v>
       </c>
       <c r="C159" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B160" s="1">
-        <v>981802</v>
+        <v>981945</v>
       </c>
       <c r="C160" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B161" s="1">
-        <v>205410</v>
+        <v>981948</v>
       </c>
       <c r="C161" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B162" s="1">
-        <v>402805</v>
+        <v>981802</v>
       </c>
       <c r="C162" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>58</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="B163" s="1">
+        <v>205410</v>
       </c>
       <c r="C163" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>239</v>
+        <v>57</v>
       </c>
       <c r="B164" s="1">
-        <v>30312</v>
+        <v>402805</v>
       </c>
       <c r="C164" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>60</v>
-      </c>
-      <c r="B165" s="1">
-        <v>70502</v>
+        <v>58</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C165" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>60</v>
+        <v>239</v>
       </c>
       <c r="B166" s="1">
-        <v>70512</v>
+        <v>30312</v>
       </c>
       <c r="C166" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>61</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>212</v>
+        <v>60</v>
+      </c>
+      <c r="B167" s="1">
+        <v>70502</v>
+      </c>
+      <c r="C167" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B168" s="1">
-        <v>1212280</v>
+        <v>70512</v>
       </c>
       <c r="C168" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C169" t="s">
-        <v>214</v>
+        <v>62</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>66</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="B170" s="1">
+        <v>1212280</v>
       </c>
       <c r="C170" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C171" s="4" t="s">
-        <v>90</v>
+        <v>65</v>
+      </c>
+      <c r="C171" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>70</v>
-      </c>
-      <c r="B172" s="1">
-        <v>1212085</v>
+        <v>66</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="C172" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>71</v>
-      </c>
-      <c r="B173" s="1">
-        <v>1212225</v>
+        <v>68</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>217</v>
+        <v>90</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>312</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>344</v>
+        <v>70</v>
+      </c>
+      <c r="B174" s="1">
+        <v>1212085</v>
+      </c>
+      <c r="C174" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>313</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>342</v>
+        <v>71</v>
+      </c>
+      <c r="B175" s="1">
+        <v>1212225</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>343</v>
+        <v>217</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>321</v>
-      </c>
-      <c r="B181" s="1">
-        <v>70680</v>
+        <v>317</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>323</v>
-      </c>
-      <c r="B182" s="1">
-        <v>14638</v>
+        <v>318</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>354</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>358</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>360</v>
+        <v>321</v>
+      </c>
+      <c r="B183" s="1">
+        <v>70680</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>323</v>
+      </c>
+      <c r="B184" s="1">
+        <v>14638</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>358</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>359</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C184" s="4" t="s">
+      <c r="C186" s="4" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>388</v>
+      </c>
+      <c r="B187" s="1">
+        <v>931167</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C84" r:id="rId2" display="https://raw.githubusercontent.com/htslabs/images/main/ 931116-PORT-E.jpg" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C81" r:id="rId3" display="https://raw.githubusercontent.com/htslabs/images/main/ 931110-SP.jpg" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C97" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C96" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C95" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C94" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C93" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C92" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C91" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C83" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C82" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C86" r:id="rId2" display="https://raw.githubusercontent.com/htslabs/images/main/ 931116-PORT-E.jpg" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C83" r:id="rId3" display="https://raw.githubusercontent.com/htslabs/images/main/ 931110-SP.jpg" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C99" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C98" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C97" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C96" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C95" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C94" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C93" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C85" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C84" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C73" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C171" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C138" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C127" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C126" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C125" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C124" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C115" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C116" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C118" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C119" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C120" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C121" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C122" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C123" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C117" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C128" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C85" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C86" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C87" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C88" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C90" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C98" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C104" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C105" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C106" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C107" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C108" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C109" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C110" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C111" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C112" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C113" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C114" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C103" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C173" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C140" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C129" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C128" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C127" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C126" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C117" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C118" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C120" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C121" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C122" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C123" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C124" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C125" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C119" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C130" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C87" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C88" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C89" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C90" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C92" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C100" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C106" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C107" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C108" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C109" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C110" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C111" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C112" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C113" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C114" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C115" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C116" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C105" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="C4" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="C5" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="C6" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
@@ -4131,30 +4188,30 @@
     <hyperlink ref="C56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="C57" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
     <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C167" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C154" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C169" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C156" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="C48" r:id="rId61" xr:uid="{5AEA7608-B58A-4A60-A4AD-2AE2F5E780E9}"/>
     <hyperlink ref="C49" r:id="rId62" xr:uid="{AFE3A760-331C-44C9-BDA1-A87C0D227BE6}"/>
-    <hyperlink ref="C173" r:id="rId63" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
-    <hyperlink ref="C174" r:id="rId64" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
-    <hyperlink ref="C175" r:id="rId65" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
-    <hyperlink ref="C176" r:id="rId66" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
-    <hyperlink ref="C177" r:id="rId67" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
-    <hyperlink ref="C178" r:id="rId68" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
-    <hyperlink ref="C179" r:id="rId69" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
-    <hyperlink ref="C180" r:id="rId70" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
+    <hyperlink ref="C175" r:id="rId63" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
+    <hyperlink ref="C176" r:id="rId64" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
+    <hyperlink ref="C177" r:id="rId65" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
+    <hyperlink ref="C178" r:id="rId66" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
+    <hyperlink ref="C179" r:id="rId67" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
+    <hyperlink ref="C180" r:id="rId68" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
+    <hyperlink ref="C181" r:id="rId69" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
+    <hyperlink ref="C182" r:id="rId70" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
     <hyperlink ref="C2" r:id="rId71" xr:uid="{55A7AC5D-4A55-40FD-B555-BF115B8C3DB2}"/>
     <hyperlink ref="C3" r:id="rId72" xr:uid="{5B2A9690-E72E-4F75-AE57-C9AB31B6BDD8}"/>
-    <hyperlink ref="C181" r:id="rId73" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
-    <hyperlink ref="C182" r:id="rId74" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
-    <hyperlink ref="C80" r:id="rId75" xr:uid="{73ED57B4-3A6D-4846-9BEA-15F1B2FCC3F8}"/>
-    <hyperlink ref="C74" r:id="rId76" xr:uid="{DD8214E1-24DE-4AF8-BCA7-B2D42CBE725C}"/>
-    <hyperlink ref="C75" r:id="rId77" xr:uid="{A5FD4093-9D9B-431D-A285-90214E03180A}"/>
-    <hyperlink ref="C76" r:id="rId78" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
-    <hyperlink ref="C77" r:id="rId79" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
-    <hyperlink ref="C78" r:id="rId80" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
-    <hyperlink ref="C183" r:id="rId81" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
-    <hyperlink ref="C184" r:id="rId82" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
+    <hyperlink ref="C183" r:id="rId73" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
+    <hyperlink ref="C184" r:id="rId74" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
+    <hyperlink ref="C81" r:id="rId75" xr:uid="{73ED57B4-3A6D-4846-9BEA-15F1B2FCC3F8}"/>
+    <hyperlink ref="C75" r:id="rId76" xr:uid="{DD8214E1-24DE-4AF8-BCA7-B2D42CBE725C}"/>
+    <hyperlink ref="C76" r:id="rId77" xr:uid="{A5FD4093-9D9B-431D-A285-90214E03180A}"/>
+    <hyperlink ref="C77" r:id="rId78" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
+    <hyperlink ref="C78" r:id="rId79" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
+    <hyperlink ref="C79" r:id="rId80" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
+    <hyperlink ref="C185" r:id="rId81" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
+    <hyperlink ref="C186" r:id="rId82" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
     <hyperlink ref="C8" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="C15" r:id="rId84" xr:uid="{D53AF88A-6A97-43F1-9E72-EFA6A2CDA035}"/>
     <hyperlink ref="C13" r:id="rId85" xr:uid="{B8D33A38-937A-4646-A6A0-6215623CD68F}"/>
@@ -4168,10 +4225,13 @@
     <hyperlink ref="C40" r:id="rId93" xr:uid="{A68412B5-9C33-485D-ADE1-B208669B4ACE}"/>
     <hyperlink ref="C41" r:id="rId94" xr:uid="{B0C47993-5B25-4EEA-AC00-BD9C1AD317C5}"/>
     <hyperlink ref="C42" r:id="rId95" xr:uid="{350F7192-A024-4641-BFDD-8597950B5A03}"/>
-    <hyperlink ref="C89" r:id="rId96" xr:uid="{67BD0A46-1F11-4E23-AC52-5E269F7F5611}"/>
-    <hyperlink ref="C79" r:id="rId97" xr:uid="{93D5D206-AF86-4AD5-9898-CDDFE15D3EC5}"/>
+    <hyperlink ref="C91" r:id="rId96" xr:uid="{67BD0A46-1F11-4E23-AC52-5E269F7F5611}"/>
+    <hyperlink ref="C80" r:id="rId97" xr:uid="{93D5D206-AF86-4AD5-9898-CDDFE15D3EC5}"/>
+    <hyperlink ref="C74" r:id="rId98" xr:uid="{59903752-97B8-4BBE-B47F-BC27D0E1C1A2}"/>
+    <hyperlink ref="C82" r:id="rId99" xr:uid="{E02C3711-CE1B-45EB-8326-CB394AD673A2}"/>
+    <hyperlink ref="C187" r:id="rId100" xr:uid="{44CE36A3-3B79-4BC3-8E95-84B1EB51EE74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId98"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId101"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
7L MP desc updated
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFEFBCB-49CC-45BD-A647-A8DCF140A46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E184B5-0D9B-4A1F-BFB5-C615F9AEDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="600" windowWidth="22575" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13080" yWindow="945" windowWidth="22575" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -1183,12 +1183,6 @@
     <t>https://raw.githubusercontent.com/htslabs/images/main/931167.jpg</t>
   </si>
   <si>
-    <t>Optimum Growth® 7L Flask w/ 1/4” Spout, Sampling Port, Sterile</t>
-  </si>
-  <si>
-    <t>Optimum Growth® 7L Flask w/ 1/8” Spout, Sampling Port, Sterile</t>
-  </si>
-  <si>
     <t>931117-55-14</t>
   </si>
   <si>
@@ -1208,6 +1202,12 @@
   </si>
   <si>
     <t>Bidirectional Transfer Cap for Optimum Growth® 7L Flask</t>
+  </si>
+  <si>
+    <t>Optimum Growth® 7L Flask w/ID 1/4” tubing from Spout &amp; Sampling Port</t>
+  </si>
+  <si>
+    <t>Optimum Growth® 7L Flask w/ID 1/8” tubing from Spout &amp; Sampling Port</t>
   </si>
 </sst>
 </file>
@@ -2078,13 +2078,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132:C132"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" customWidth="1"/>
+    <col min="1" max="1" width="79.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="72.85546875" customWidth="1"/>
   </cols>
@@ -2905,24 +2905,24 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>394</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C75" s="4" t="s">
         <v>389</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>395</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3532,13 +3532,13 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 6-well and inline filter
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E184B5-0D9B-4A1F-BFB5-C615F9AEDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB848033-199F-4263-ACA2-865D329E35D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="945" windowWidth="22575" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9615" yWindow="765" windowWidth="28230" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="401">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -1208,6 +1208,21 @@
   </si>
   <si>
     <t>Optimum Growth® 7L Flask w/ID 1/8” tubing from Spout &amp; Sampling Port</t>
+  </si>
+  <si>
+    <t>Optimum Growth® Integrated Lid for 6-Well</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/981648.jpg</t>
+  </si>
+  <si>
+    <t>761050-10</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/761050-10.jpg</t>
+  </si>
+  <si>
+    <t>50mm Inline Filter</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:C76"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,6 +4181,28 @@
       </c>
       <c r="C189" s="4" t="s">
         <v>386</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>396</v>
+      </c>
+      <c r="B190" s="1">
+        <v>981648</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>400</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -4272,8 +4309,10 @@
     <hyperlink ref="C75" r:id="rId100" xr:uid="{F9D2ED08-FBF3-4AAC-A896-EDE0456263F3}"/>
     <hyperlink ref="C76" r:id="rId101" xr:uid="{DD55D42C-BE09-4597-91E1-A055B4693D5E}"/>
     <hyperlink ref="C132" r:id="rId102" xr:uid="{6FD09735-42C0-4297-8661-70E4A723CF74}"/>
+    <hyperlink ref="C190" r:id="rId103" xr:uid="{82E375B1-E256-4F1C-941F-18CD2654EB52}"/>
+    <hyperlink ref="C191" r:id="rId104" xr:uid="{A7AF95C3-A193-4105-83FE-C1054001F63A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId103"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId105"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uploading -DP's with tubing
</commit_message>
<xml_diff>
--- a/website_products_URLimages.xlsx
+++ b/website_products_URLimages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklotz\Documents\DAMR\Thomson Marketing\Dan\__Websites\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thomsoninstrumentcompany-my.sharepoint.com/personal/dklotz_htslabs_com/Documents/Documents/DAMR/Thomson Marketing/Dan/__Websites/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F126729E-B885-4294-9CE5-C948D7C8A56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{F126729E-B885-4294-9CE5-C948D7C8A56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E680485-295A-4C03-BBA6-49C59D653321}"/>
   <bookViews>
-    <workbookView xWindow="8430" yWindow="1035" windowWidth="24105" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12930" yWindow="795" windowWidth="25170" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_URLimages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="406">
   <si>
     <t>Toggle Press</t>
   </si>
@@ -1220,6 +1220,24 @@
   </si>
   <si>
     <t>50mm Inline Filter</t>
+  </si>
+  <si>
+    <t>Multiported Optimum Growth® 125mL Flask (image with tubing attached)</t>
+  </si>
+  <si>
+    <t>Multiported Optimum Growth® 250mL Flask (image with tubing attached)</t>
+  </si>
+  <si>
+    <t>Multiported Optimum Growth® 500mL Flask (image with tubing attached)</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931110-DP-tube.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931111-D-tubeP.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/htslabs/images/main/931112-DP-tube.jpg</t>
   </si>
 </sst>
 </file>
@@ -2088,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,299 +3089,299 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>278</v>
+        <v>400</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>106</v>
+        <v>403</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>280</v>
+        <v>401</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>108</v>
+        <v>404</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>376</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>375</v>
+        <v>279</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>377</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>281</v>
+        <v>402</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>109</v>
+        <v>405</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>16</v>
-      </c>
-      <c r="B94" s="1">
-        <v>1212900</v>
+        <v>280</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>17</v>
-      </c>
-      <c r="B95" s="1">
-        <v>1212905</v>
+        <v>376</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>375</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>85</v>
+        <v>377</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>282</v>
-      </c>
-      <c r="B96" s="1">
-        <v>899110</v>
+        <v>281</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>283</v>
+        <v>16</v>
       </c>
       <c r="B97" s="1">
-        <v>899111</v>
+        <v>1212900</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="B98" s="1">
-        <v>899112</v>
+        <v>1212905</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B99" s="1">
-        <v>899116</v>
+        <v>899110</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>286</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>79</v>
+        <v>283</v>
+      </c>
+      <c r="B100" s="1">
+        <v>899111</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>18</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>19</v>
+        <v>284</v>
+      </c>
+      <c r="B101" s="1">
+        <v>899112</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B102" s="1">
-        <v>788116</v>
-      </c>
-      <c r="C102" t="s">
-        <v>170</v>
+        <v>899116</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>288</v>
-      </c>
-      <c r="B103" s="1">
-        <v>931147</v>
-      </c>
-      <c r="C103" t="s">
-        <v>171</v>
+        <v>286</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>289</v>
-      </c>
-      <c r="B104" s="1">
-        <v>931144</v>
-      </c>
-      <c r="C104" t="s">
-        <v>172</v>
+        <v>18</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B105" s="1">
-        <v>931141</v>
+        <v>788116</v>
       </c>
       <c r="C105" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B106" s="1">
-        <v>931138</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>120</v>
+        <v>931147</v>
+      </c>
+      <c r="C106" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>292</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>111</v>
+        <v>289</v>
+      </c>
+      <c r="B107" s="1">
+        <v>931144</v>
+      </c>
+      <c r="C107" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B108" s="1">
-        <v>899136</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>112</v>
+        <v>931141</v>
+      </c>
+      <c r="C108" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B109" s="1">
-        <v>899109</v>
+        <v>931138</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>295</v>
-      </c>
-      <c r="B110" s="1">
-        <v>899110</v>
+        <v>292</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B111" s="1">
-        <v>899111</v>
+        <v>899136</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B112" s="1">
-        <v>899566</v>
+        <v>899109</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B113" s="1">
-        <v>899421</v>
+        <v>899110</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B114" s="1">
-        <v>899423</v>
+        <v>899111</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B115" s="1">
-        <v>899424</v>
+        <v>899566</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3371,54 +3389,54 @@
         <v>298</v>
       </c>
       <c r="B116" s="1">
-        <v>899425</v>
+        <v>899421</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B117" s="1">
-        <v>446300</v>
+        <v>899423</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>300</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>21</v>
+        <v>298</v>
+      </c>
+      <c r="B118" s="1">
+        <v>899424</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>300</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>22</v>
+        <v>298</v>
+      </c>
+      <c r="B119" s="1">
+        <v>899425</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>300</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>23</v>
+        <v>299</v>
+      </c>
+      <c r="B120" s="1">
+        <v>446300</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3426,43 +3444,43 @@
         <v>300</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3470,10 +3488,10 @@
         <v>301</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3481,285 +3499,285 @@
         <v>301</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>392</v>
+        <v>303</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>390</v>
+        <v>32</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>391</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>305</v>
-      </c>
-      <c r="B133" s="1">
-        <v>931609</v>
-      </c>
-      <c r="C133" t="s">
-        <v>174</v>
+        <v>304</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>306</v>
-      </c>
-      <c r="B134" s="1">
-        <v>931700</v>
-      </c>
-      <c r="C134" t="s">
-        <v>175</v>
+        <v>304</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>307</v>
-      </c>
-      <c r="B135" s="1">
-        <v>931606</v>
-      </c>
-      <c r="C135" t="s">
-        <v>176</v>
+        <v>392</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B136" s="1">
-        <v>931607</v>
+        <v>931609</v>
       </c>
       <c r="C136" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>35</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>36</v>
+        <v>306</v>
+      </c>
+      <c r="B137" s="1">
+        <v>931700</v>
       </c>
       <c r="C137" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>35</v>
+        <v>307</v>
       </c>
       <c r="B138" s="1">
-        <v>931568</v>
+        <v>931606</v>
       </c>
       <c r="C138" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>37</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>38</v>
+        <v>308</v>
+      </c>
+      <c r="B139" s="1">
+        <v>931607</v>
       </c>
       <c r="C139" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>37</v>
-      </c>
-      <c r="B140" s="1">
-        <v>931571</v>
+        <v>35</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C140" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B141" s="1">
-        <v>951657</v>
+        <v>931568</v>
       </c>
       <c r="C141" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>182</v>
+        <v>38</v>
+      </c>
+      <c r="C142" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B143" s="1">
-        <v>931130</v>
+        <v>931571</v>
       </c>
       <c r="C143" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>39</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>41</v>
+      <c r="B144" s="1">
+        <v>951657</v>
       </c>
       <c r="C144" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>236</v>
+        <v>39</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C145" t="s">
-        <v>185</v>
+        <v>40</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>237</v>
+        <v>39</v>
       </c>
       <c r="B146" s="1">
-        <v>9356045</v>
+        <v>931130</v>
       </c>
       <c r="C146" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>39</v>
       </c>
-      <c r="B147" s="1">
-        <v>931133</v>
+      <c r="B147" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C147" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>39</v>
-      </c>
-      <c r="B148" s="1">
-        <v>931137</v>
+        <v>236</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C148" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>43</v>
+        <v>237</v>
       </c>
       <c r="B149" s="1">
-        <v>931919</v>
+        <v>9356045</v>
       </c>
       <c r="C149" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B150" s="1">
-        <v>921746</v>
+        <v>931133</v>
       </c>
       <c r="C150" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B151" s="1">
-        <v>921730</v>
+        <v>931137</v>
       </c>
       <c r="C151" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3767,10 +3785,10 @@
         <v>43</v>
       </c>
       <c r="B152" s="1">
-        <v>921740</v>
+        <v>931919</v>
       </c>
       <c r="C152" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3778,427 +3796,460 @@
         <v>43</v>
       </c>
       <c r="B153" s="1">
-        <v>921731</v>
+        <v>921746</v>
       </c>
       <c r="C153" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B154" s="1">
-        <v>921550</v>
+        <v>921730</v>
       </c>
       <c r="C154" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B155" s="1">
-        <v>921546</v>
+        <v>921740</v>
       </c>
       <c r="C155" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B156" s="1">
-        <v>359747</v>
+        <v>921731</v>
       </c>
       <c r="C156" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>46</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B157" s="1">
+        <v>921550</v>
       </c>
       <c r="C157" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>48</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>198</v>
+        <v>45</v>
+      </c>
+      <c r="B158" s="1">
+        <v>921546</v>
+      </c>
+      <c r="C158" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B159" s="1">
-        <v>899410</v>
+        <v>359747</v>
       </c>
       <c r="C159" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>51</v>
-      </c>
-      <c r="B160" s="1">
-        <v>899403</v>
+        <v>46</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C160" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>52</v>
-      </c>
-      <c r="B161" s="1">
-        <v>899406</v>
-      </c>
-      <c r="C161" t="s">
-        <v>201</v>
+        <v>48</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B162" s="1">
-        <v>981945</v>
+        <v>899410</v>
       </c>
       <c r="C162" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B163" s="1">
-        <v>981948</v>
+        <v>899403</v>
       </c>
       <c r="C163" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B164" s="1">
-        <v>981802</v>
+        <v>899406</v>
       </c>
       <c r="C164" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B165" s="1">
-        <v>205410</v>
+        <v>981945</v>
       </c>
       <c r="C165" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B166" s="1">
-        <v>402805</v>
+        <v>981948</v>
       </c>
       <c r="C166" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>58</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B167" s="1">
+        <v>981802</v>
       </c>
       <c r="C167" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>238</v>
+        <v>56</v>
       </c>
       <c r="B168" s="1">
-        <v>30312</v>
+        <v>205410</v>
       </c>
       <c r="C168" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B169" s="1">
-        <v>70502</v>
+        <v>402805</v>
       </c>
       <c r="C169" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>60</v>
-      </c>
-      <c r="B170" s="1">
-        <v>70512</v>
+        <v>58</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C170" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>61</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C171" s="4" t="s">
-        <v>211</v>
+        <v>238</v>
+      </c>
+      <c r="B171" s="1">
+        <v>30312</v>
+      </c>
+      <c r="C171" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B172" s="1">
-        <v>1212280</v>
+        <v>70502</v>
       </c>
       <c r="C172" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>64</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="B173" s="1">
+        <v>70512</v>
       </c>
       <c r="C173" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C174" t="s">
-        <v>214</v>
+        <v>62</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>68</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C175" s="4" t="s">
-        <v>90</v>
+        <v>63</v>
+      </c>
+      <c r="B175" s="1">
+        <v>1212280</v>
+      </c>
+      <c r="C175" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>70</v>
-      </c>
-      <c r="B176" s="1">
-        <v>1212085</v>
+        <v>64</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C176" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>71</v>
-      </c>
-      <c r="B177" s="1">
-        <v>1212225</v>
-      </c>
-      <c r="C177" s="4" t="s">
-        <v>216</v>
+        <v>66</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C177" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>311</v>
+        <v>68</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>344</v>
+        <v>69</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>343</v>
+        <v>90</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>312</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C179" s="4" t="s">
-        <v>342</v>
+        <v>70</v>
+      </c>
+      <c r="B179" s="1">
+        <v>1212085</v>
+      </c>
+      <c r="C179" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>313</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>347</v>
+        <v>71</v>
+      </c>
+      <c r="B180" s="1">
+        <v>1212225</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>348</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>320</v>
-      </c>
-      <c r="B185" s="1">
-        <v>70680</v>
+        <v>315</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>322</v>
-      </c>
-      <c r="B186" s="1">
-        <v>14638</v>
+        <v>316</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>358</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>360</v>
+        <v>320</v>
+      </c>
+      <c r="B188" s="1">
+        <v>70680</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>362</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>384</v>
+        <v>322</v>
       </c>
       <c r="B189" s="1">
-        <v>931167</v>
+        <v>14638</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>385</v>
+        <v>323</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>395</v>
-      </c>
-      <c r="B190" s="1">
-        <v>981648</v>
+        <v>357</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>396</v>
+        <v>361</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>358</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>384</v>
+      </c>
+      <c r="B192" s="1">
+        <v>931167</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>395</v>
+      </c>
+      <c r="B193" s="1">
+        <v>981648</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>399</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B194" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="C191" s="4" t="s">
+      <c r="C194" s="4" t="s">
         <v>398</v>
       </c>
     </row>
@@ -4207,50 +4258,50 @@
     <hyperlink ref="C52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C87" r:id="rId2" display="https://raw.githubusercontent.com/htslabs/images/main/ 931116-PORT-E.jpg" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C84" r:id="rId3" display="https://raw.githubusercontent.com/htslabs/images/main/ 931110-SP.jpg" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C100" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C99" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C98" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C97" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C96" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C95" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C94" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C103" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C102" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C101" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C100" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C99" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C98" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C97" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="C86" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="C85" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C73" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C175" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C142" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C130" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C129" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C128" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C127" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C118" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C119" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C121" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C122" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C123" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C124" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C125" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C126" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C120" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C131" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C178" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C145" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C133" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C132" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C131" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C130" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C121" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C122" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C124" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C125" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C126" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C127" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C128" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C129" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C123" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C134" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="C88" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C89" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C90" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C91" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C93" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C101" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C107" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C108" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C109" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C110" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C111" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C112" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C113" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C114" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C115" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C116" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C117" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C106" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C90" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C92" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C94" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C96" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C104" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C110" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C111" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C112" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C113" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C114" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C115" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C116" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C117" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C118" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C119" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C120" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C109" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="C4" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="C5" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="C6" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
@@ -4262,30 +4313,30 @@
     <hyperlink ref="C56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="C57" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
     <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C171" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C158" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C174" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C161" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="C48" r:id="rId61" xr:uid="{5AEA7608-B58A-4A60-A4AD-2AE2F5E780E9}"/>
     <hyperlink ref="C49" r:id="rId62" xr:uid="{AFE3A760-331C-44C9-BDA1-A87C0D227BE6}"/>
-    <hyperlink ref="C177" r:id="rId63" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
-    <hyperlink ref="C178" r:id="rId64" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
-    <hyperlink ref="C179" r:id="rId65" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
-    <hyperlink ref="C180" r:id="rId66" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
-    <hyperlink ref="C181" r:id="rId67" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
-    <hyperlink ref="C182" r:id="rId68" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
-    <hyperlink ref="C183" r:id="rId69" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
-    <hyperlink ref="C184" r:id="rId70" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
+    <hyperlink ref="C180" r:id="rId63" xr:uid="{F106C974-2FCE-4A37-AF72-2DE5B907E068}"/>
+    <hyperlink ref="C181" r:id="rId64" xr:uid="{38E0CCED-C7EF-4526-8F98-209BE28F4617}"/>
+    <hyperlink ref="C182" r:id="rId65" xr:uid="{0F90CDF1-38E9-4993-A104-B823B148E4EA}"/>
+    <hyperlink ref="C183" r:id="rId66" xr:uid="{396F9F8A-F02E-41D0-82BA-38B542BC8AA5}"/>
+    <hyperlink ref="C184" r:id="rId67" xr:uid="{B46CE9F9-1A26-4532-853C-D69D01225766}"/>
+    <hyperlink ref="C185" r:id="rId68" xr:uid="{347628F6-CEDD-4C6D-B93F-4ED4588CDBDA}"/>
+    <hyperlink ref="C186" r:id="rId69" xr:uid="{68622522-96A6-4727-9141-092B60304BAC}"/>
+    <hyperlink ref="C187" r:id="rId70" xr:uid="{0CADF770-BD51-4BC1-8089-DB7E258F5EBA}"/>
     <hyperlink ref="C2" r:id="rId71" xr:uid="{55A7AC5D-4A55-40FD-B555-BF115B8C3DB2}"/>
     <hyperlink ref="C3" r:id="rId72" xr:uid="{5B2A9690-E72E-4F75-AE57-C9AB31B6BDD8}"/>
-    <hyperlink ref="C185" r:id="rId73" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
-    <hyperlink ref="C186" r:id="rId74" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
+    <hyperlink ref="C188" r:id="rId73" xr:uid="{A5F66F02-088A-4104-9CCB-6E40BDA0017E}"/>
+    <hyperlink ref="C189" r:id="rId74" xr:uid="{BBFD54D5-4A29-40BE-BE33-5C03D8E0C802}"/>
     <hyperlink ref="C83" r:id="rId75" xr:uid="{73ED57B4-3A6D-4846-9BEA-15F1B2FCC3F8}"/>
     <hyperlink ref="C77" r:id="rId76" xr:uid="{DD8214E1-24DE-4AF8-BCA7-B2D42CBE725C}"/>
     <hyperlink ref="C78" r:id="rId77" xr:uid="{A5FD4093-9D9B-431D-A285-90214E03180A}"/>
     <hyperlink ref="C79" r:id="rId78" xr:uid="{80C70727-430D-48B5-95C9-84219B181A25}"/>
     <hyperlink ref="C80" r:id="rId79" xr:uid="{1BBE61C7-10F4-44D8-9376-0ED9B594DFCE}"/>
     <hyperlink ref="C81" r:id="rId80" xr:uid="{DA863CEA-E773-432F-BAB0-485918CEEBE2}"/>
-    <hyperlink ref="C187" r:id="rId81" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
-    <hyperlink ref="C188" r:id="rId82" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
+    <hyperlink ref="C190" r:id="rId81" xr:uid="{13760E9A-9130-44D1-A833-538D4A8CA4BE}"/>
+    <hyperlink ref="C191" r:id="rId82" xr:uid="{7798F13D-B97E-412C-B328-E5EA74345F0E}"/>
     <hyperlink ref="C8" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="C15" r:id="rId84" xr:uid="{D53AF88A-6A97-43F1-9E72-EFA6A2CDA035}"/>
     <hyperlink ref="C13" r:id="rId85" xr:uid="{B8D33A38-937A-4646-A6A0-6215623CD68F}"/>
@@ -4299,17 +4350,20 @@
     <hyperlink ref="C40" r:id="rId93" xr:uid="{A68412B5-9C33-485D-ADE1-B208669B4ACE}"/>
     <hyperlink ref="C41" r:id="rId94" xr:uid="{B0C47993-5B25-4EEA-AC00-BD9C1AD317C5}"/>
     <hyperlink ref="C42" r:id="rId95" xr:uid="{350F7192-A024-4641-BFDD-8597950B5A03}"/>
-    <hyperlink ref="C92" r:id="rId96" xr:uid="{67BD0A46-1F11-4E23-AC52-5E269F7F5611}"/>
+    <hyperlink ref="C95" r:id="rId96" xr:uid="{67BD0A46-1F11-4E23-AC52-5E269F7F5611}"/>
     <hyperlink ref="C82" r:id="rId97" xr:uid="{93D5D206-AF86-4AD5-9898-CDDFE15D3EC5}"/>
     <hyperlink ref="C74" r:id="rId98" xr:uid="{59903752-97B8-4BBE-B47F-BC27D0E1C1A2}"/>
-    <hyperlink ref="C189" r:id="rId99" xr:uid="{44CE36A3-3B79-4BC3-8E95-84B1EB51EE74}"/>
+    <hyperlink ref="C192" r:id="rId99" xr:uid="{44CE36A3-3B79-4BC3-8E95-84B1EB51EE74}"/>
     <hyperlink ref="C75" r:id="rId100" xr:uid="{F9D2ED08-FBF3-4AAC-A896-EDE0456263F3}"/>
     <hyperlink ref="C76" r:id="rId101" xr:uid="{DD55D42C-BE09-4597-91E1-A055B4693D5E}"/>
-    <hyperlink ref="C132" r:id="rId102" xr:uid="{6FD09735-42C0-4297-8661-70E4A723CF74}"/>
-    <hyperlink ref="C190" r:id="rId103" xr:uid="{82E375B1-E256-4F1C-941F-18CD2654EB52}"/>
-    <hyperlink ref="C191" r:id="rId104" xr:uid="{A7AF95C3-A193-4105-83FE-C1054001F63A}"/>
+    <hyperlink ref="C135" r:id="rId102" xr:uid="{6FD09735-42C0-4297-8661-70E4A723CF74}"/>
+    <hyperlink ref="C193" r:id="rId103" xr:uid="{82E375B1-E256-4F1C-941F-18CD2654EB52}"/>
+    <hyperlink ref="C194" r:id="rId104" xr:uid="{A7AF95C3-A193-4105-83FE-C1054001F63A}"/>
+    <hyperlink ref="C89" r:id="rId105" xr:uid="{26D2BD6E-8D75-4A67-925B-0C3DC95F45B2}"/>
+    <hyperlink ref="C91" r:id="rId106" xr:uid="{AA3B0F77-8D65-43D4-A4C3-72EE153922ED}"/>
+    <hyperlink ref="C93" r:id="rId107" xr:uid="{F0241F35-E016-4479-8DF5-ECEF49937029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId105"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId108"/>
 </worksheet>
 </file>
</xml_diff>